<commit_message>
New files with flask application
</commit_message>
<xml_diff>
--- a/rules.xlsx
+++ b/rules.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\College\College\DAB - 103\Fun Proj\dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC80D9FE-8A16-4EAF-B4E1-EBC71A0DF0BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07125D1-E983-4AFF-B8AD-1557D75950D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3732" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="rule_desc" sheetId="1" r:id="rId1"/>
+    <sheet name="id_1" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,21 +26,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Rule No.</t>
-  </si>
-  <si>
-    <t>Quiz - 1% to 4%</t>
-  </si>
-  <si>
-    <t>Test - 5% to 24%</t>
-  </si>
-  <si>
-    <t>Exam 25% to 40%</t>
-  </si>
-  <si>
-    <t>Assessment Rule</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>rule_func()</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t>rule_1(page1)</t>
+  </si>
+  <si>
+    <t>rule_2_cd(page1)</t>
+  </si>
+  <si>
+    <t>rule_2_pd(page1)</t>
+  </si>
+  <si>
+    <t>rule_2_ad(page1)</t>
+  </si>
+  <si>
+    <t>Displays if any of the assessment is breaching its expected weightage in the syllabus</t>
+  </si>
+  <si>
+    <t>Displays verb distance of EKS and CLO based on cognitive domain word list</t>
+  </si>
+  <si>
+    <t>Displays verb distance of EKS and CLO based on psychomotor domain word list</t>
+  </si>
+  <si>
+    <t>Displays verb distance of EKS and CLO based on affective domain word list</t>
+  </si>
+  <si>
+    <t>lower</t>
+  </si>
+  <si>
+    <t>higher</t>
+  </si>
+  <si>
+    <t>assessment</t>
+  </si>
+  <si>
+    <t>Quiz</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Exam</t>
+  </si>
+  <si>
+    <t>Quiz weightage should be between 1% to 4%</t>
+  </si>
+  <si>
+    <t>Test weightage should be between 5% to 24%</t>
+  </si>
+  <si>
+    <t>Exam weightage should be between 25% to 40%</t>
+  </si>
+  <si>
+    <t>rules</t>
   </si>
 </sst>
 </file>
@@ -92,6 +141,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{243678A6-D28F-4AFB-9B08-51BB60D22B89}" name="Table3" displayName="Table3" ref="A1:D4" totalsRowShown="0">
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{D0180976-1CC0-4DA2-9B19-71072CC54620}" name="assessment"/>
+    <tableColumn id="2" xr3:uid="{8423EDB4-EEA9-42BB-BF3D-E00684787719}" name="lower"/>
+    <tableColumn id="3" xr3:uid="{61A7F771-46C7-414B-9694-BA63EFAE9517}" name="higher"/>
+    <tableColumn id="4" xr3:uid="{FACA170A-D3F1-411E-B54B-CAAF0B6AE78E}" name="rules"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -357,47 +418,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="54.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E87878-014B-47C0-A571-DEF94A370B7D}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="40.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>